<commit_message>
Merged user profile and clean up
</commit_message>
<xml_diff>
--- a/emma_albert/Insert Multi Rows.xlsx
+++ b/emma_albert/Insert Multi Rows.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="query" sheetId="1" r:id="rId1"/>
@@ -26,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="91">
-  <si>
-    <t>test_user</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="126">
   <si>
     <t>2016-04-11 09:00:00</t>
   </si>
@@ -46,9 +43,6 @@
     <t>http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg</t>
   </si>
   <si>
-    <t>test_agent</t>
-  </si>
-  <si>
     <t>-33.7687822,150.904815</t>
   </si>
   <si>
@@ -97,18 +91,9 @@
     <t>When does the next train to the city come?</t>
   </si>
   <si>
-    <t>test_agent2</t>
-  </si>
-  <si>
-    <t>user</t>
-  </si>
-  <si>
     <t>tester</t>
   </si>
   <si>
-    <t>password</t>
-  </si>
-  <si>
     <t>APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzSu</t>
   </si>
   <si>
@@ -130,9 +115,6 @@
     <t>albbui@gmail.com</t>
   </si>
   <si>
-    <t>2016-03-01</t>
-  </si>
-  <si>
     <t>user2</t>
   </si>
   <si>
@@ -299,6 +281,129 @@
   </si>
   <si>
     <t>2016-04-01</t>
+  </si>
+  <si>
+    <t>2016-04-11 08:10:04</t>
+  </si>
+  <si>
+    <t>2016-04-11 08:10:05</t>
+  </si>
+  <si>
+    <t>2016-04-11 08:10:06</t>
+  </si>
+  <si>
+    <t>2016-04-11 08:10:07</t>
+  </si>
+  <si>
+    <t>2016-04-11 08:10:08</t>
+  </si>
+  <si>
+    <t>2016-04-11 08:10:09</t>
+  </si>
+  <si>
+    <t>2016-04-11 07:10:10</t>
+  </si>
+  <si>
+    <t>2016-04-11 07:10:11</t>
+  </si>
+  <si>
+    <t>2016-04-11 07:10:12</t>
+  </si>
+  <si>
+    <t>2016-04-11 07:10:13</t>
+  </si>
+  <si>
+    <t>2016-04-11 07:10:14</t>
+  </si>
+  <si>
+    <t>2016-04-11 07:10:15</t>
+  </si>
+  <si>
+    <t>2016-04-11 06:10:16</t>
+  </si>
+  <si>
+    <t>2016-04-11 06:10:17</t>
+  </si>
+  <si>
+    <t>2016-04-11 06:10:18</t>
+  </si>
+  <si>
+    <t>2016-04-11 06:10:19</t>
+  </si>
+  <si>
+    <t>2016-04-11 06:10:20</t>
+  </si>
+  <si>
+    <t>agent1</t>
+  </si>
+  <si>
+    <t>agent2</t>
+  </si>
+  <si>
+    <t>agent3</t>
+  </si>
+  <si>
+    <t>user6</t>
+  </si>
+  <si>
+    <t>user7</t>
+  </si>
+  <si>
+    <t>agent4</t>
+  </si>
+  <si>
+    <t>agent5</t>
+  </si>
+  <si>
+    <t>Ryan</t>
+  </si>
+  <si>
+    <t>Ken</t>
+  </si>
+  <si>
+    <t>amosangyj@gmail.com</t>
+  </si>
+  <si>
+    <t>kens23@gmail.com</t>
+  </si>
+  <si>
+    <t>ryan.arsenna@gmail.com</t>
+  </si>
+  <si>
+    <t>2016-04-02</t>
+  </si>
+  <si>
+    <t>2016-04-03</t>
+  </si>
+  <si>
+    <t>2016-04-04</t>
+  </si>
+  <si>
+    <t>2016-04-09</t>
+  </si>
+  <si>
+    <t>APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS6</t>
+  </si>
+  <si>
+    <t>0498745632</t>
+  </si>
+  <si>
+    <t>0498745633</t>
+  </si>
+  <si>
+    <t>0498745634</t>
+  </si>
+  <si>
+    <t>0498745635</t>
+  </si>
+  <si>
+    <t>0498745636</t>
+  </si>
+  <si>
+    <t>0498745637</t>
+  </si>
+  <si>
+    <t>0498745638</t>
   </si>
 </sst>
 </file>
@@ -628,10 +733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="E20" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:M41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,42 +759,42 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="I1" t="s">
-        <v>6</v>
+        <v>102</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="K1">
         <v>2</v>
       </c>
       <c r="L1" t="str">
-        <f>"INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES ("</f>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (</v>
+        <f>"INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES ("</f>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M1" t="str">
         <f>L1 &amp; A1 &amp; ",'" &amp; B1 &amp; "','" &amp; C1 &amp; "','" &amp; D1 &amp; "','" &amp; E1 &amp; "','" &amp; F1 &amp; "','" &amp; G1 &amp; "','" &amp; H1 &amp; "','" &amp; I1 &amp; "','" &amp; J1 &amp; "'," &amp; K1 &amp; ");"</f>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (1,'test_user','2016-04-11 09:00:00','-33.7687822,150.904814','how tall is michael jordan','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','1.98m','test_agent','2016-04-11 09:10:20',2);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (1,'user7','2016-04-11 09:00:00','-33.7687822,150.904814','how tall is michael jordan','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','1.98m','agent1','2016-04-11 09:10:20',2);</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -697,42 +802,42 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="I2" t="s">
-        <v>6</v>
+        <v>102</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="K2">
         <v>2</v>
       </c>
       <c r="L2" t="str">
-        <f t="shared" ref="L2:L21" si="0">"INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES ("</f>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (</v>
+        <f t="shared" ref="L2:L41" si="0">"INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES ("</f>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M2" t="str">
-        <f t="shared" ref="M2:M21" si="1">L2 &amp; A2 &amp; ",'" &amp; B2 &amp; "','" &amp; C2 &amp; "','" &amp; D2 &amp; "','" &amp; E2 &amp; "','" &amp; F2 &amp; "','" &amp; G2 &amp; "','" &amp; H2 &amp; "','" &amp; I2 &amp; "','" &amp; J2 &amp; "'," &amp; K2 &amp; ");"</f>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (2,'test_user','2016-04-11 09:05:01','-33.7687822,150.904815','how tall is barack obama','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','1.85m','test_agent','2016-04-11 09:10:21',2);</v>
+        <f t="shared" ref="M2:M41" si="1">L2 &amp; A2 &amp; ",'" &amp; B2 &amp; "','" &amp; C2 &amp; "','" &amp; D2 &amp; "','" &amp; E2 &amp; "','" &amp; F2 &amp; "','" &amp; G2 &amp; "','" &amp; H2 &amp; "','" &amp; I2 &amp; "','" &amp; J2 &amp; "'," &amp; K2 &amp; ");"</f>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (2,'user7','2016-04-11 09:05:01','-33.7687822,150.904815','how tall is barack obama','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','1.85m','agent1','2016-04-11 09:10:21',2);</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -740,42 +845,42 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="I3" t="s">
-        <v>6</v>
+        <v>102</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="K3">
         <v>2</v>
       </c>
       <c r="L3" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (3,'test_user','2016-04-11 09:10:02','-33.7687822,150.904816','how old is hillary clinton','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','68 years','test_agent','2016-04-11 09:10:22',2);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (3,'user7','2016-04-11 09:10:02','-33.7687822,150.904816','how old is hillary clinton','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','68 years','agent1','2016-04-11 09:10:22',2);</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -783,42 +888,42 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H4" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="I4" t="s">
-        <v>6</v>
+        <v>102</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K4">
         <v>2</v>
       </c>
       <c r="L4" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M4" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (4,'test_user','2016-04-11 09:10:03','-33.7687822,150.904814','how tall is napolean bonaparte','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','1.69m','test_agent','2016-04-11 09:10:23',2);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (4,'user7','2016-04-11 09:10:03','-33.7687822,150.904814','how tall is napolean bonaparte','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','1.69m','agent1','2016-04-11 09:10:23',2);</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -826,42 +931,42 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
       <c r="L5" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M5" t="str">
-        <f>L5 &amp; A5 &amp; ",'" &amp; B5 &amp; "','" &amp; C5 &amp; "','" &amp; D5 &amp; "','" &amp; E5 &amp; "','" &amp; F5 &amp; "','" &amp; G5 &amp; "'," &amp; H5 &amp; "," &amp; I5 &amp; "," &amp; J5 &amp; "," &amp; K5 &amp; ");"</f>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (5,'test_user','2016-04-11 09:10:04','-33.7687822,150.904814','how tall is buzz aldrin','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (5,'user7','2016-04-11 09:10:04','-33.7687822,150.904814','how tall is buzz aldrin','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -869,42 +974,42 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
       <c r="L6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M6" t="str">
-        <f t="shared" ref="M6:M21" si="2">L6 &amp; A6 &amp; ",'" &amp; B6 &amp; "','" &amp; C6 &amp; "','" &amp; D6 &amp; "','" &amp; E6 &amp; "','" &amp; F6 &amp; "','" &amp; G6 &amp; "'," &amp; H6 &amp; "," &amp; I6 &amp; "," &amp; J6 &amp; "," &amp; K6 &amp; ");"</f>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (6,'test_user','2016-04-11 09:10:05','-33.7687822,150.904814','how tall is adolf hitler','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (6,'user7','2016-04-11 09:10:05','-33.7687822,150.904814','how tall is adolf hitler','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -912,42 +1017,42 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K7">
         <v>0</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M7" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (7,'test_user','2016-04-11 09:10:06','-33.7687822,150.904814','how tall is stalin','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (7,'user7','2016-04-11 09:10:06','-33.7687822,150.904814','how tall is stalin','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -955,42 +1060,42 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M8" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (8,'test_user','2016-04-11 09:10:07','-33.7687822,150.904814','how tall is shaquille oneal','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (8,'user7','2016-04-11 09:10:07','-33.7687822,150.904814','how tall is shaquille oneal','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -998,42 +1103,42 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K9">
         <v>0</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M9" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (9,'test_user','2016-04-11 09:10:08','-33.7687822,150.904814','how tall is bill clinton','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (9,'user7','2016-04-11 09:10:08','-33.7687822,150.904814','how tall is bill clinton','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -1041,42 +1146,42 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M10" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (10,'test_user','2016-04-11 09:10:09','-33.7687822,150.904814','how tall is michelle obama','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (10,'user7','2016-04-11 09:10:09','-33.7687822,150.904814','how tall is michelle obama','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -1084,42 +1189,42 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D11" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M11" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (11,'test_user','2016-04-11 09:10:10','-33.7687822,150.904814','How far is my closest train station?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (11,'user7','2016-04-11 09:10:10','-33.7687822,150.904814','How far is my closest train station?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -1127,42 +1232,42 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K12">
         <v>0</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M12" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (12,'test_user','2016-04-11 09:10:11','-33.7687822,150.904814','When does the next train to the city come?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (12,'user7','2016-04-11 09:10:11','-33.7687822,150.904814','When does the next train to the city come?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -1170,42 +1275,42 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K13">
         <v>0</v>
       </c>
       <c r="L13" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M13" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (13,'test_user','2016-04-11 09:10:12','-33.7687822,150.904814','How long will it take me to walk there?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (13,'user7','2016-04-11 09:10:12','-33.7687822,150.904814','How long will it take me to walk there?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -1213,42 +1318,42 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K14">
         <v>0</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M14" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (14,'test_user','2016-04-11 09:10:13','-33.7687822,150.904814','What time does the train get to Melbourne Central?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (14,'user7','2016-04-11 09:10:13','-33.7687822,150.904814','What time does the train get to Melbourne Central?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -1256,42 +1361,42 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K15">
         <v>0</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M15" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (15,'test_user','2016-04-11 09:10:14','-33.7687822,150.904814','Are there any screenings of Batman vs Superman tonight?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (15,'user7','2016-04-11 09:10:14','-33.7687822,150.904814','Are there any screenings of Batman vs Superman tonight?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -1299,42 +1404,42 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D16" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K16">
         <v>0</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M16" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (16,'test_user','2016-04-11 09:10:15','-33.7687822,150.904814','Can you please book 2 tickets for me?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (16,'user7','2016-04-11 09:10:15','-33.7687822,150.904814','Can you please book 2 tickets for me?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -1342,42 +1447,42 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D17" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K17">
         <v>0</v>
       </c>
       <c r="L17" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M17" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (17,'test_user','2016-04-11 09:10:16','-33.7687822,150.904814','Where is a good place to have Japanese food for dinner nearby?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (17,'user7','2016-04-11 09:10:16','-33.7687822,150.904814','Where is a good place to have Japanese food for dinner nearby?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -1385,42 +1490,42 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K18">
         <v>0</v>
       </c>
       <c r="L18" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M18" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (18,'test_user','2016-04-11 09:10:17','-33.7687822,150.904814','Can you make a reservation for me before the movie?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (18,'user7','2016-04-11 09:10:17','-33.7687822,150.904814','Can you make a reservation for me before the movie?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -1428,42 +1533,42 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D19" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K19">
         <v>0</v>
       </c>
       <c r="L19" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M19" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (19,'test_user','2016-04-11 09:10:18','-33.7687822,150.904814','What time does Myer close tonight?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (19,'user7','2016-04-11 09:10:18','-33.7687822,150.904814','What time does Myer close tonight?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -1471,42 +1576,42 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D20" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K20">
         <v>0</v>
       </c>
       <c r="L20" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M20" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (20,'test_user','2016-04-11 09:10:19','-33.7687822,150.904814','Should I bring an umbrella?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (20,'user7','2016-04-11 09:10:19','-33.7687822,150.904814','Should I bring an umbrella?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -1514,42 +1619,773 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>78</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H21" t="s">
+        <v>19</v>
+      </c>
+      <c r="I21" t="s">
+        <v>19</v>
+      </c>
+      <c r="J21" t="s">
+        <v>19</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
+      </c>
+      <c r="M21" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (21,'user7','2016-04-11 09:10:20','-33.7687822,150.904814','Anything else to do in the city after the movie?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H23" t="s">
+        <v>19</v>
+      </c>
+      <c r="I23" t="s">
+        <v>19</v>
+      </c>
+      <c r="J23" t="s">
+        <v>19</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
+      </c>
+      <c r="M23" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (23,'user1','2016-04-11 08:10:04','-33.7687822,150.904814','how tall is buzz aldrin','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H24" t="s">
+        <v>19</v>
+      </c>
+      <c r="I24" t="s">
+        <v>19</v>
+      </c>
+      <c r="J24" t="s">
+        <v>19</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
+      </c>
+      <c r="M24" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (24,'user1','2016-04-11 08:10:05','-33.7687822,150.904814','how tall is adolf hitler','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H25" t="s">
+        <v>19</v>
+      </c>
+      <c r="I25" t="s">
+        <v>19</v>
+      </c>
+      <c r="J25" t="s">
+        <v>19</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
+      </c>
+      <c r="M25" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (25,'user1','2016-04-11 08:10:06','-33.7687822,150.904814','how tall is stalin','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>26</v>
+      </c>
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H26" t="s">
+        <v>19</v>
+      </c>
+      <c r="I26" t="s">
+        <v>19</v>
+      </c>
+      <c r="J26" t="s">
+        <v>19</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
+      </c>
+      <c r="M26" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (26,'user1','2016-04-11 08:10:07','-33.7687822,150.904814','how tall is shaquille oneal','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H27" t="s">
+        <v>19</v>
+      </c>
+      <c r="I27" t="s">
+        <v>19</v>
+      </c>
+      <c r="J27" t="s">
+        <v>19</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
+      </c>
+      <c r="M27" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (27,'user1','2016-04-11 08:10:08','-33.7687822,150.904814','how tall is bill clinton','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H28" t="s">
+        <v>19</v>
+      </c>
+      <c r="I28" t="s">
+        <v>19</v>
+      </c>
+      <c r="J28" t="s">
+        <v>19</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
+      </c>
+      <c r="M28" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (28,'user1','2016-04-11 08:10:09','-33.7687822,150.904814','how tall is michelle obama','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
+        <v>16</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H30" t="s">
+        <v>19</v>
+      </c>
+      <c r="I30" t="s">
+        <v>19</v>
+      </c>
+      <c r="J30" t="s">
+        <v>19</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
+      </c>
+      <c r="M30" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (30,'user2','2016-04-11 07:10:10','-33.7687822,150.904814','How far is my closest train station?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>31</v>
+      </c>
+      <c r="B31" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
+        <v>20</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H31" t="s">
+        <v>19</v>
+      </c>
+      <c r="I31" t="s">
+        <v>19</v>
+      </c>
+      <c r="J31" t="s">
+        <v>19</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
+      </c>
+      <c r="M31" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (31,'user2','2016-04-11 07:10:11','-33.7687822,150.904814','When does the next train to the city come?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>32</v>
+      </c>
+      <c r="B32" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D32" t="s">
+        <v>1</v>
+      </c>
+      <c r="E32" t="s">
+        <v>70</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H32" t="s">
+        <v>19</v>
+      </c>
+      <c r="I32" t="s">
+        <v>19</v>
+      </c>
+      <c r="J32" t="s">
+        <v>19</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
+      </c>
+      <c r="M32" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (32,'user2','2016-04-11 07:10:12','-33.7687822,150.904814','How long will it take me to walk there?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>33</v>
+      </c>
+      <c r="B33" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1</v>
+      </c>
+      <c r="E33" t="s">
+        <v>71</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H33" t="s">
+        <v>19</v>
+      </c>
+      <c r="I33" t="s">
+        <v>19</v>
+      </c>
+      <c r="J33" t="s">
+        <v>19</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
+      </c>
+      <c r="M33" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (33,'user2','2016-04-11 07:10:13','-33.7687822,150.904814','What time does the train get to Melbourne Central?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>34</v>
+      </c>
+      <c r="B34" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D34" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
         <v>72</v>
       </c>
-      <c r="D21" t="s">
-        <v>2</v>
-      </c>
-      <c r="E21" t="s">
-        <v>84</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H21" t="s">
-        <v>21</v>
-      </c>
-      <c r="I21" t="s">
-        <v>21</v>
-      </c>
-      <c r="J21" t="s">
-        <v>21</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (</v>
-      </c>
-      <c r="M21" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, answeredby, answertime, status) VALUES (21,'test_user','2016-04-11 09:10:20','-33.7687822,150.904814','Anything else to do in the city after the movie?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+      <c r="F34" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H34" t="s">
+        <v>19</v>
+      </c>
+      <c r="I34" t="s">
+        <v>19</v>
+      </c>
+      <c r="J34" t="s">
+        <v>19</v>
+      </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
+      <c r="L34" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
+      </c>
+      <c r="M34" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (34,'user2','2016-04-11 07:10:14','-33.7687822,150.904814','Are there any screenings of Batman vs Superman tonight?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>35</v>
+      </c>
+      <c r="B35" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D35" t="s">
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
+        <v>73</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H35" t="s">
+        <v>19</v>
+      </c>
+      <c r="I35" t="s">
+        <v>19</v>
+      </c>
+      <c r="J35" t="s">
+        <v>19</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
+      </c>
+      <c r="M35" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (35,'user2','2016-04-11 07:10:15','-33.7687822,150.904814','Can you please book 2 tickets for me?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>37</v>
+      </c>
+      <c r="B37" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D37" t="s">
+        <v>1</v>
+      </c>
+      <c r="E37" t="s">
+        <v>74</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H37" t="s">
+        <v>19</v>
+      </c>
+      <c r="I37" t="s">
+        <v>19</v>
+      </c>
+      <c r="J37" t="s">
+        <v>19</v>
+      </c>
+      <c r="K37">
+        <v>0</v>
+      </c>
+      <c r="L37" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
+      </c>
+      <c r="M37" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (37,'user3','2016-04-11 06:10:16','-33.7687822,150.904814','Where is a good place to have Japanese food for dinner nearby?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>38</v>
+      </c>
+      <c r="B38" t="s">
+        <v>31</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D38" t="s">
+        <v>1</v>
+      </c>
+      <c r="E38" t="s">
+        <v>75</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H38" t="s">
+        <v>19</v>
+      </c>
+      <c r="I38" t="s">
+        <v>19</v>
+      </c>
+      <c r="J38" t="s">
+        <v>19</v>
+      </c>
+      <c r="K38">
+        <v>0</v>
+      </c>
+      <c r="L38" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
+      </c>
+      <c r="M38" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (38,'user3','2016-04-11 06:10:17','-33.7687822,150.904814','Can you make a reservation for me before the movie?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>39</v>
+      </c>
+      <c r="B39" t="s">
+        <v>31</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D39" t="s">
+        <v>1</v>
+      </c>
+      <c r="E39" t="s">
+        <v>76</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H39" t="s">
+        <v>19</v>
+      </c>
+      <c r="I39" t="s">
+        <v>19</v>
+      </c>
+      <c r="J39" t="s">
+        <v>19</v>
+      </c>
+      <c r="K39">
+        <v>0</v>
+      </c>
+      <c r="L39" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
+      </c>
+      <c r="M39" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (39,'user3','2016-04-11 06:10:18','-33.7687822,150.904814','What time does Myer close tonight?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>40</v>
+      </c>
+      <c r="B40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D40" t="s">
+        <v>1</v>
+      </c>
+      <c r="E40" t="s">
+        <v>77</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H40" t="s">
+        <v>19</v>
+      </c>
+      <c r="I40" t="s">
+        <v>19</v>
+      </c>
+      <c r="J40" t="s">
+        <v>19</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+      <c r="L40" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
+      </c>
+      <c r="M40" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (40,'user3','2016-04-11 06:10:19','-33.7687822,150.904814','Should I bring an umbrella?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>41</v>
+      </c>
+      <c r="B41" t="s">
+        <v>31</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D41" t="s">
+        <v>1</v>
+      </c>
+      <c r="E41" t="s">
+        <v>78</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H41" t="s">
+        <v>19</v>
+      </c>
+      <c r="I41" t="s">
+        <v>19</v>
+      </c>
+      <c r="J41" t="s">
+        <v>19</v>
+      </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
+      <c r="L41" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
+      </c>
+      <c r="M41" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (41,'user3','2016-04-11 06:10:20','-33.7687822,150.904814','Anything else to do in the city after the movie?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
       </c>
     </row>
   </sheetData>
@@ -1595,364 +2431,514 @@
     <hyperlink ref="F19" r:id="rId39"/>
     <hyperlink ref="F20" r:id="rId40"/>
     <hyperlink ref="F21" r:id="rId41"/>
+    <hyperlink ref="F23:F26" r:id="rId42" display="http://www.soundjay.com/misc/bell-ringing-01.mp3"/>
+    <hyperlink ref="G23" r:id="rId43"/>
+    <hyperlink ref="G24" r:id="rId44"/>
+    <hyperlink ref="G25" r:id="rId45"/>
+    <hyperlink ref="G26" r:id="rId46"/>
+    <hyperlink ref="G27" r:id="rId47"/>
+    <hyperlink ref="G28" r:id="rId48"/>
+    <hyperlink ref="F23" r:id="rId49"/>
+    <hyperlink ref="F24" r:id="rId50"/>
+    <hyperlink ref="F25" r:id="rId51"/>
+    <hyperlink ref="F26" r:id="rId52"/>
+    <hyperlink ref="F27" r:id="rId53"/>
+    <hyperlink ref="F28" r:id="rId54"/>
+    <hyperlink ref="G30" r:id="rId55"/>
+    <hyperlink ref="G31" r:id="rId56"/>
+    <hyperlink ref="G32" r:id="rId57"/>
+    <hyperlink ref="G33" r:id="rId58"/>
+    <hyperlink ref="G34" r:id="rId59"/>
+    <hyperlink ref="G35" r:id="rId60"/>
+    <hyperlink ref="F30" r:id="rId61"/>
+    <hyperlink ref="F31" r:id="rId62"/>
+    <hyperlink ref="F32" r:id="rId63"/>
+    <hyperlink ref="F33" r:id="rId64"/>
+    <hyperlink ref="F34" r:id="rId65"/>
+    <hyperlink ref="F35" r:id="rId66"/>
+    <hyperlink ref="G37" r:id="rId67"/>
+    <hyperlink ref="G38" r:id="rId68"/>
+    <hyperlink ref="G39" r:id="rId69"/>
+    <hyperlink ref="G40" r:id="rId70"/>
+    <hyperlink ref="G41" r:id="rId71"/>
+    <hyperlink ref="F37" r:id="rId72"/>
+    <hyperlink ref="F38" r:id="rId73"/>
+    <hyperlink ref="F39" r:id="rId74"/>
+    <hyperlink ref="F40" r:id="rId75"/>
+    <hyperlink ref="F41" r:id="rId76"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId42"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId77"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>102</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1">
-        <v>470449425</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
       </c>
       <c r="H1">
         <v>0</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="J1" t="str">
         <f>"INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('"</f>
         <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('</v>
       </c>
       <c r="K1" t="str">
-        <f>J1 &amp; A1 &amp; "','" &amp; B1 &amp; "'," &amp; C1 &amp; ",'" &amp; D1 &amp; "','" &amp; E1 &amp; "','" &amp; F1 &amp; "','" &amp; G1 &amp; "'," &amp; H1 &amp; ",'" &amp; I1 &amp; "');"</f>
-        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('test_agent','tester',NULL,'Sanjeev','me_sanjeev@hotmail.com','470449425','2016-03-01',0,'2016-04-01');</v>
+        <f>J1 &amp; A1 &amp; "','" &amp; B1 &amp; "'," &amp; C1 &amp; ",'" &amp; D1 &amp; "','" &amp; E1 &amp; "'," &amp; F1 &amp; "," &amp; G1 &amp; "," &amp; H1 &amp; ",'" &amp; I1 &amp; "');"</f>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('agent1','tester',NULL,'Sanjeev','me_sanjeev@hotmail.com',NULL,NULL,0,'2016-04-01');</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" t="s">
-        <v>21</v>
+        <v>25</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="J2" t="str">
-        <f t="shared" ref="J2:J9" si="0">"INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('"</f>
+        <f t="shared" ref="J2:J12" si="0">"INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('"</f>
         <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('</v>
       </c>
       <c r="K2" t="str">
-        <f>J2 &amp; A2 &amp; "'," &amp; B2 &amp; "," &amp; C2 &amp; ",'" &amp; D2 &amp; "'," &amp; E2 &amp; "," &amp; F2 &amp; "," &amp; G2 &amp; "," &amp; H2 &amp; ",'" &amp; I2 &amp; "');"</f>
-        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('test_user',NULL,NULL,'John',NULL,NULL,NULL,1,'2016-04-01');</v>
+        <f t="shared" ref="K2:K5" si="1">J2 &amp; A2 &amp; "','" &amp; B2 &amp; "'," &amp; C2 &amp; ",'" &amp; D2 &amp; "','" &amp; E2 &amp; "'," &amp; F2 &amp; "," &amp; G2 &amp; "," &amp; H2 &amp; ",'" &amp; I2 &amp; "');"</f>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('agent2','tester',NULL,'Albert','albbui@gmail.com',NULL,NULL,0,'2016-04-01');</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>104</v>
       </c>
       <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" t="s">
-        <v>30</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3">
-        <v>1234</v>
+        <v>111</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="J3" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('</v>
       </c>
       <c r="K3" t="str">
-        <f>J3 &amp; A3 &amp; "','" &amp; B3 &amp; "'," &amp; C3 &amp; ",'" &amp; D3 &amp; "','" &amp; E3 &amp; "','" &amp; F3 &amp; "'," &amp; G3 &amp; "," &amp; H3 &amp; ",'" &amp; I3 &amp; "');"</f>
-        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('test_agent2','password',NULL,'Albert','albbui@gmail.com','1234',NULL,0,'2016-04-01');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('agent3','tester',NULL,'Amos','amosangyj@gmail.com',NULL,NULL,0,'2016-04-02');</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>107</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" t="s">
-        <v>27</v>
+      <c r="C4" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4">
-        <v>5678</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>34</v>
+        <v>109</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="J4" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('</v>
       </c>
       <c r="K4" t="str">
-        <f>J4 &amp; A4 &amp; "'," &amp; B4 &amp; ",'" &amp; C4 &amp; "','" &amp; D4 &amp; "'," &amp; E4 &amp; ",'" &amp; F4 &amp; "','" &amp; G4 &amp; "'," &amp; H4 &amp; ",'" &amp; I4 &amp; "');"</f>
-        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('user',NULL,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzSu','Amos',NULL,'5678','2016-03-01',1,'2016-04-01');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('agent4','tester',NULL,'Ryan','ryan.arsenna@gmail.com',NULL,NULL,0,'2016-04-03');</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>108</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" t="s">
-        <v>40</v>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
+        <v>110</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>50</v>
+        <v>116</v>
       </c>
       <c r="J5" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('</v>
       </c>
       <c r="K5" t="str">
-        <f>J5 &amp; A5 &amp; "'," &amp; B5 &amp; ",'" &amp; C5 &amp; "','" &amp; D5 &amp; "'," &amp; E5 &amp; "," &amp; F5 &amp; "," &amp; G5 &amp; "," &amp; H5 &amp; ",'" &amp; I5 &amp; "');"</f>
-        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('user1',NULL,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS1','Josh',NULL,NULL,NULL,1,'2016-04-10');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('agent5','tester',NULL,'Ken','kens23@gmail.com',NULL,NULL,0,'2016-04-04');</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>119</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H6">
         <v>1</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>51</v>
+        <v>117</v>
       </c>
       <c r="J6" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('</v>
       </c>
       <c r="K6" t="str">
-        <f t="shared" ref="K6:K9" si="1">J6 &amp; A6 &amp; "'," &amp; B6 &amp; ",'" &amp; C6 &amp; "','" &amp; D6 &amp; "'," &amp; E6 &amp; "," &amp; F6 &amp; "," &amp; G6 &amp; "," &amp; H6 &amp; ",'" &amp; I6 &amp; "');"</f>
-        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('user2',NULL,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS2','Mary',NULL,NULL,NULL,1,'2016-04-11');</v>
+        <f>J6 &amp; A6 &amp; "'," &amp; B6 &amp; ",'" &amp; C6 &amp; "','" &amp; D6 &amp; "'," &amp; E6 &amp; ",'" &amp; F6 &amp; "'," &amp; G6 &amp; "," &amp; H6 &amp; ",'" &amp; I6 &amp; "');"</f>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('user1',NULL,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzSu','Amos',NULL,'0498745632',NULL,1,'2016-04-09');</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>120</v>
       </c>
       <c r="G7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H7">
         <v>1</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="J7" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('</v>
       </c>
       <c r="K7" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('user3',NULL,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS3','Bob',NULL,NULL,NULL,1,'2016-04-12');</v>
+        <f t="shared" ref="K7:K12" si="2">J7 &amp; A7 &amp; "'," &amp; B7 &amp; ",'" &amp; C7 &amp; "','" &amp; D7 &amp; "'," &amp; E7 &amp; ",'" &amp; F7 &amp; "'," &amp; G7 &amp; "," &amp; H7 &amp; ",'" &amp; I7 &amp; "');"</f>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('user2',NULL,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS1','Josh',NULL,'0498745633',NULL,1,'2016-04-10');</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>121</v>
       </c>
       <c r="G8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="J8" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('</v>
       </c>
       <c r="K8" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('user4',NULL,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS4','Jack',NULL,NULL,NULL,1,'2016-04-13');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('user3',NULL,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS2','Mary',NULL,'0498745634',NULL,1,'2016-04-11');</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>122</v>
       </c>
       <c r="G9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H9">
         <v>1</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="J9" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('</v>
       </c>
       <c r="K9" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('user5',NULL,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS5','Juliet',NULL,NULL,NULL,1,'2016-04-14');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('user4',NULL,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS3','Bob',NULL,'0498745635',NULL,1,'2016-04-12');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('user5',NULL,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS4','Jack',NULL,'0498745636',NULL,1,'2016-04-13');</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('user6',NULL,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS5','Juliet',NULL,'0498745637',NULL,1,'2016-04-14');</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>118</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('user7',NULL,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS6','John',NULL,'0498745638',NULL,1,'2016-04-01');</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E1" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="E3" r:id="rId3"/>
+    <hyperlink ref="E5" r:id="rId4"/>
+    <hyperlink ref="E4" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1973,52 +2959,52 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented a working fix to get google results to display. Removed Load Google button
</commit_message>
<xml_diff>
--- a/emma_albert/Insert Multi Rows.xlsx
+++ b/emma_albert/Insert Multi Rows.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\emma_refactored\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\emma_albert\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="query" sheetId="1" r:id="rId1"/>
@@ -733,10 +733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M41"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E20" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:M41"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D34" sqref="A34:XFD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,11 +832,11 @@
         <v>2</v>
       </c>
       <c r="L2" t="str">
-        <f t="shared" ref="L2:L41" si="0">"INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES ("</f>
+        <f t="shared" ref="L2:L38" si="0">"INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES ("</f>
         <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M2" t="str">
-        <f t="shared" ref="M2:M41" si="1">L2 &amp; A2 &amp; ",'" &amp; B2 &amp; "','" &amp; C2 &amp; "','" &amp; D2 &amp; "','" &amp; E2 &amp; "','" &amp; F2 &amp; "','" &amp; G2 &amp; "','" &amp; H2 &amp; "','" &amp; I2 &amp; "','" &amp; J2 &amp; "'," &amp; K2 &amp; ");"</f>
+        <f t="shared" ref="M2:M4" si="1">L2 &amp; A2 &amp; ",'" &amp; B2 &amp; "','" &amp; C2 &amp; "','" &amp; D2 &amp; "','" &amp; E2 &amp; "','" &amp; F2 &amp; "','" &amp; G2 &amp; "','" &amp; H2 &amp; "','" &amp; I2 &amp; "','" &amp; J2 &amp; "'," &amp; K2 &amp; ");"</f>
         <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (2,'user7','2016-04-11 09:05:01','-33.7687822,150.904815','how tall is barack obama','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','1.85m','agent1','2016-04-11 09:10:21',2);</v>
       </c>
     </row>
@@ -965,8 +965,8 @@
         <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M5" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (5,'user7','2016-04-11 09:10:04','-33.7687822,150.904814','how tall is buzz aldrin','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+        <f>L5 &amp; A5 &amp; ",'" &amp; B5 &amp; "','" &amp; C5 &amp; "','" &amp; D5 &amp; "','" &amp; E5 &amp; "','" &amp; F5 &amp; "','" &amp; G5 &amp; "'," &amp; H5 &amp; "," &amp; I5 &amp; "," &amp; J5 &amp; "," &amp; K5 &amp; ");"</f>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (5,'user7','2016-04-11 09:10:04','-33.7687822,150.904814','how tall is buzz aldrin','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1008,8 +1008,8 @@
         <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M6" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (6,'user7','2016-04-11 09:10:05','-33.7687822,150.904814','how tall is adolf hitler','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+        <f t="shared" ref="M6:M38" si="2">L6 &amp; A6 &amp; ",'" &amp; B6 &amp; "','" &amp; C6 &amp; "','" &amp; D6 &amp; "','" &amp; E6 &amp; "','" &amp; F6 &amp; "','" &amp; G6 &amp; "'," &amp; H6 &amp; "," &amp; I6 &amp; "," &amp; J6 &amp; "," &amp; K6 &amp; ");"</f>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (6,'user7','2016-04-11 09:10:05','-33.7687822,150.904814','how tall is adolf hitler','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1051,8 +1051,8 @@
         <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M7" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (7,'user7','2016-04-11 09:10:06','-33.7687822,150.904814','how tall is stalin','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (7,'user7','2016-04-11 09:10:06','-33.7687822,150.904814','how tall is stalin','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1094,8 +1094,8 @@
         <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M8" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (8,'user7','2016-04-11 09:10:07','-33.7687822,150.904814','how tall is shaquille oneal','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (8,'user7','2016-04-11 09:10:07','-33.7687822,150.904814','how tall is shaquille oneal','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1137,8 +1137,8 @@
         <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M9" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (9,'user7','2016-04-11 09:10:08','-33.7687822,150.904814','how tall is bill clinton','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (9,'user7','2016-04-11 09:10:08','-33.7687822,150.904814','how tall is bill clinton','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -1180,8 +1180,8 @@
         <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M10" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (10,'user7','2016-04-11 09:10:09','-33.7687822,150.904814','how tall is michelle obama','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (10,'user7','2016-04-11 09:10:09','-33.7687822,150.904814','how tall is michelle obama','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -1223,8 +1223,8 @@
         <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M11" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (11,'user7','2016-04-11 09:10:10','-33.7687822,150.904814','How far is my closest train station?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (11,'user7','2016-04-11 09:10:10','-33.7687822,150.904814','How far is my closest train station?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -1266,8 +1266,8 @@
         <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M12" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (12,'user7','2016-04-11 09:10:11','-33.7687822,150.904814','When does the next train to the city come?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (12,'user7','2016-04-11 09:10:11','-33.7687822,150.904814','When does the next train to the city come?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -1309,8 +1309,8 @@
         <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M13" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (13,'user7','2016-04-11 09:10:12','-33.7687822,150.904814','How long will it take me to walk there?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (13,'user7','2016-04-11 09:10:12','-33.7687822,150.904814','How long will it take me to walk there?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -1352,8 +1352,8 @@
         <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M14" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (14,'user7','2016-04-11 09:10:13','-33.7687822,150.904814','What time does the train get to Melbourne Central?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (14,'user7','2016-04-11 09:10:13','-33.7687822,150.904814','What time does the train get to Melbourne Central?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -1395,8 +1395,8 @@
         <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M15" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (15,'user7','2016-04-11 09:10:14','-33.7687822,150.904814','Are there any screenings of Batman vs Superman tonight?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (15,'user7','2016-04-11 09:10:14','-33.7687822,150.904814','Are there any screenings of Batman vs Superman tonight?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -1438,8 +1438,8 @@
         <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M16" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (16,'user7','2016-04-11 09:10:15','-33.7687822,150.904814','Can you please book 2 tickets for me?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (16,'user7','2016-04-11 09:10:15','-33.7687822,150.904814','Can you please book 2 tickets for me?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -1481,8 +1481,8 @@
         <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M17" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (17,'user7','2016-04-11 09:10:16','-33.7687822,150.904814','Where is a good place to have Japanese food for dinner nearby?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (17,'user7','2016-04-11 09:10:16','-33.7687822,150.904814','Where is a good place to have Japanese food for dinner nearby?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -1524,8 +1524,8 @@
         <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M18" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (18,'user7','2016-04-11 09:10:17','-33.7687822,150.904814','Can you make a reservation for me before the movie?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (18,'user7','2016-04-11 09:10:17','-33.7687822,150.904814','Can you make a reservation for me before the movie?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -1567,8 +1567,8 @@
         <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M19" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (19,'user7','2016-04-11 09:10:18','-33.7687822,150.904814','What time does Myer close tonight?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (19,'user7','2016-04-11 09:10:18','-33.7687822,150.904814','What time does Myer close tonight?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -1610,8 +1610,8 @@
         <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M20" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (20,'user7','2016-04-11 09:10:19','-33.7687822,150.904814','Should I bring an umbrella?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (20,'user7','2016-04-11 09:10:19','-33.7687822,150.904814','Should I bring an umbrella?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -1653,25 +1653,68 @@
         <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M21" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (21,'user7','2016-04-11 09:10:20','-33.7687822,150.904814','Anything else to do in the city after the movie?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (21,'user7','2016-04-11 09:10:20','-33.7687822,150.904814','Anything else to do in the city after the movie?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H22" t="s">
+        <v>19</v>
+      </c>
+      <c r="I22" t="s">
+        <v>19</v>
+      </c>
+      <c r="J22" t="s">
+        <v>19</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
+      </c>
+      <c r="M22" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (23,'user1','2016-04-11 08:10:04','-33.7687822,150.904814','how tall is buzz aldrin','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
         <v>30</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D23" t="s">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>3</v>
@@ -1696,25 +1739,25 @@
         <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M23" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (23,'user1','2016-04-11 08:10:04','-33.7687822,150.904814','how tall is buzz aldrin','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (24,'user1','2016-04-11 08:10:05','-33.7687822,150.904814','how tall is adolf hitler','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
         <v>30</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D24" t="s">
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>3</v>
@@ -1739,25 +1782,25 @@
         <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M24" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (24,'user1','2016-04-11 08:10:05','-33.7687822,150.904814','how tall is adolf hitler','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (25,'user1','2016-04-11 08:10:06','-33.7687822,150.904814','how tall is stalin','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B25" t="s">
         <v>30</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D25" t="s">
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>3</v>
@@ -1782,25 +1825,25 @@
         <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M25" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (25,'user1','2016-04-11 08:10:06','-33.7687822,150.904814','how tall is stalin','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (26,'user1','2016-04-11 08:10:07','-33.7687822,150.904814','how tall is shaquille oneal','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B26" t="s">
         <v>30</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D26" t="s">
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>3</v>
@@ -1825,25 +1868,25 @@
         <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M26" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (26,'user1','2016-04-11 08:10:07','-33.7687822,150.904814','how tall is shaquille oneal','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (27,'user1','2016-04-11 08:10:08','-33.7687822,150.904814','how tall is bill clinton','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B27" t="s">
         <v>30</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D27" t="s">
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>3</v>
@@ -1868,25 +1911,25 @@
         <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M27" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (27,'user1','2016-04-11 08:10:08','-33.7687822,150.904814','how tall is bill clinton','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (28,'user1','2016-04-11 08:10:09','-33.7687822,150.904814','how tall is michelle obama','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D28" t="s">
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>3</v>
@@ -1911,25 +1954,68 @@
         <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M28" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (28,'user1','2016-04-11 08:10:09','-33.7687822,150.904814','how tall is michelle obama','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (30,'user2','2016-04-11 07:10:10','-33.7687822,150.904814','How far is my closest train station?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>31</v>
+      </c>
+      <c r="B29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>20</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H29" t="s">
+        <v>19</v>
+      </c>
+      <c r="I29" t="s">
+        <v>19</v>
+      </c>
+      <c r="J29" t="s">
+        <v>19</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
+      </c>
+      <c r="M29" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (31,'user2','2016-04-11 07:10:11','-33.7687822,150.904814','When does the next train to the city come?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B30" t="s">
         <v>29</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D30" t="s">
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>16</v>
+        <v>70</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>3</v>
@@ -1954,25 +2040,25 @@
         <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M30" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (30,'user2','2016-04-11 07:10:10','-33.7687822,150.904814','How far is my closest train station?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (32,'user2','2016-04-11 07:10:12','-33.7687822,150.904814','How long will it take me to walk there?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B31" t="s">
         <v>29</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D31" t="s">
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>20</v>
+        <v>71</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>3</v>
@@ -1997,25 +2083,25 @@
         <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M31" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (31,'user2','2016-04-11 07:10:11','-33.7687822,150.904814','When does the next train to the city come?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (33,'user2','2016-04-11 07:10:13','-33.7687822,150.904814','What time does the train get to Melbourne Central?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B32" t="s">
         <v>29</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D32" t="s">
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>3</v>
@@ -2040,25 +2126,25 @@
         <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M32" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (32,'user2','2016-04-11 07:10:12','-33.7687822,150.904814','How long will it take me to walk there?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (34,'user2','2016-04-11 07:10:14','-33.7687822,150.904814','Are there any screenings of Batman vs Superman tonight?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B33" t="s">
         <v>29</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D33" t="s">
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>3</v>
@@ -2083,25 +2169,25 @@
         <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M33" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (33,'user2','2016-04-11 07:10:13','-33.7687822,150.904814','What time does the train get to Melbourne Central?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (35,'user2','2016-04-11 07:10:15','-33.7687822,150.904814','Can you please book 2 tickets for me?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D34" t="s">
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>3</v>
@@ -2126,25 +2212,25 @@
         <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M34" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (34,'user2','2016-04-11 07:10:14','-33.7687822,150.904814','Are there any screenings of Batman vs Superman tonight?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (37,'user3','2016-04-11 06:10:16','-33.7687822,150.904814','Where is a good place to have Japanese food for dinner nearby?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B35" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D35" t="s">
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>3</v>
@@ -2169,25 +2255,68 @@
         <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M35" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (35,'user2','2016-04-11 07:10:15','-33.7687822,150.904814','Can you please book 2 tickets for me?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (38,'user3','2016-04-11 06:10:17','-33.7687822,150.904814','Can you make a reservation for me before the movie?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>39</v>
+      </c>
+      <c r="B36" t="s">
+        <v>31</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D36" t="s">
+        <v>1</v>
+      </c>
+      <c r="E36" t="s">
+        <v>76</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H36" t="s">
+        <v>19</v>
+      </c>
+      <c r="I36" t="s">
+        <v>19</v>
+      </c>
+      <c r="J36" t="s">
+        <v>19</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+      <c r="L36" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
+      </c>
+      <c r="M36" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (39,'user3','2016-04-11 06:10:18','-33.7687822,150.904814','What time does Myer close tonight?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B37" t="s">
         <v>31</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D37" t="s">
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>3</v>
@@ -2212,25 +2341,25 @@
         <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M37" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (37,'user3','2016-04-11 06:10:16','-33.7687822,150.904814','Where is a good place to have Japanese food for dinner nearby?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (40,'user3','2016-04-11 06:10:19','-33.7687822,150.904814','Should I bring an umbrella?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B38" t="s">
         <v>31</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D38" t="s">
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>3</v>
@@ -2255,137 +2384,8 @@
         <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M38" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (38,'user3','2016-04-11 06:10:17','-33.7687822,150.904814','Can you make a reservation for me before the movie?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>39</v>
-      </c>
-      <c r="B39" t="s">
-        <v>31</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D39" t="s">
-        <v>1</v>
-      </c>
-      <c r="E39" t="s">
-        <v>76</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H39" t="s">
-        <v>19</v>
-      </c>
-      <c r="I39" t="s">
-        <v>19</v>
-      </c>
-      <c r="J39" t="s">
-        <v>19</v>
-      </c>
-      <c r="K39">
-        <v>0</v>
-      </c>
-      <c r="L39" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
-      </c>
-      <c r="M39" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (39,'user3','2016-04-11 06:10:18','-33.7687822,150.904814','What time does Myer close tonight?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>40</v>
-      </c>
-      <c r="B40" t="s">
-        <v>31</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D40" t="s">
-        <v>1</v>
-      </c>
-      <c r="E40" t="s">
-        <v>77</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H40" t="s">
-        <v>19</v>
-      </c>
-      <c r="I40" t="s">
-        <v>19</v>
-      </c>
-      <c r="J40" t="s">
-        <v>19</v>
-      </c>
-      <c r="K40">
-        <v>0</v>
-      </c>
-      <c r="L40" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
-      </c>
-      <c r="M40" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (40,'user3','2016-04-11 06:10:19','-33.7687822,150.904814','Should I bring an umbrella?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>41</v>
-      </c>
-      <c r="B41" t="s">
-        <v>31</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D41" t="s">
-        <v>1</v>
-      </c>
-      <c r="E41" t="s">
-        <v>78</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H41" t="s">
-        <v>19</v>
-      </c>
-      <c r="I41" t="s">
-        <v>19</v>
-      </c>
-      <c r="J41" t="s">
-        <v>19</v>
-      </c>
-      <c r="K41">
-        <v>0</v>
-      </c>
-      <c r="L41" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
-      </c>
-      <c r="M41" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (41,'user3','2016-04-11 06:10:20','-33.7687822,150.904814','Anything else to do in the city after the movie?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','NULL','NULL','NULL',0);</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (41,'user3','2016-04-11 06:10:20','-33.7687822,150.904814','Anything else to do in the city after the movie?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
   </sheetData>
@@ -2431,41 +2431,41 @@
     <hyperlink ref="F19" r:id="rId39"/>
     <hyperlink ref="F20" r:id="rId40"/>
     <hyperlink ref="F21" r:id="rId41"/>
-    <hyperlink ref="F23:F26" r:id="rId42" display="http://www.soundjay.com/misc/bell-ringing-01.mp3"/>
-    <hyperlink ref="G23" r:id="rId43"/>
-    <hyperlink ref="G24" r:id="rId44"/>
-    <hyperlink ref="G25" r:id="rId45"/>
-    <hyperlink ref="G26" r:id="rId46"/>
-    <hyperlink ref="G27" r:id="rId47"/>
-    <hyperlink ref="G28" r:id="rId48"/>
-    <hyperlink ref="F23" r:id="rId49"/>
-    <hyperlink ref="F24" r:id="rId50"/>
-    <hyperlink ref="F25" r:id="rId51"/>
-    <hyperlink ref="F26" r:id="rId52"/>
-    <hyperlink ref="F27" r:id="rId53"/>
-    <hyperlink ref="F28" r:id="rId54"/>
-    <hyperlink ref="G30" r:id="rId55"/>
-    <hyperlink ref="G31" r:id="rId56"/>
-    <hyperlink ref="G32" r:id="rId57"/>
-    <hyperlink ref="G33" r:id="rId58"/>
-    <hyperlink ref="G34" r:id="rId59"/>
-    <hyperlink ref="G35" r:id="rId60"/>
-    <hyperlink ref="F30" r:id="rId61"/>
-    <hyperlink ref="F31" r:id="rId62"/>
-    <hyperlink ref="F32" r:id="rId63"/>
-    <hyperlink ref="F33" r:id="rId64"/>
-    <hyperlink ref="F34" r:id="rId65"/>
-    <hyperlink ref="F35" r:id="rId66"/>
-    <hyperlink ref="G37" r:id="rId67"/>
-    <hyperlink ref="G38" r:id="rId68"/>
-    <hyperlink ref="G39" r:id="rId69"/>
-    <hyperlink ref="G40" r:id="rId70"/>
-    <hyperlink ref="G41" r:id="rId71"/>
-    <hyperlink ref="F37" r:id="rId72"/>
-    <hyperlink ref="F38" r:id="rId73"/>
-    <hyperlink ref="F39" r:id="rId74"/>
-    <hyperlink ref="F40" r:id="rId75"/>
-    <hyperlink ref="F41" r:id="rId76"/>
+    <hyperlink ref="F22:F25" r:id="rId42" display="http://www.soundjay.com/misc/bell-ringing-01.mp3"/>
+    <hyperlink ref="G22" r:id="rId43"/>
+    <hyperlink ref="G23" r:id="rId44"/>
+    <hyperlink ref="G24" r:id="rId45"/>
+    <hyperlink ref="G25" r:id="rId46"/>
+    <hyperlink ref="G26" r:id="rId47"/>
+    <hyperlink ref="G27" r:id="rId48"/>
+    <hyperlink ref="F22" r:id="rId49"/>
+    <hyperlink ref="F23" r:id="rId50"/>
+    <hyperlink ref="F24" r:id="rId51"/>
+    <hyperlink ref="F25" r:id="rId52"/>
+    <hyperlink ref="F26" r:id="rId53"/>
+    <hyperlink ref="F27" r:id="rId54"/>
+    <hyperlink ref="G28" r:id="rId55"/>
+    <hyperlink ref="G29" r:id="rId56"/>
+    <hyperlink ref="G30" r:id="rId57"/>
+    <hyperlink ref="G31" r:id="rId58"/>
+    <hyperlink ref="G32" r:id="rId59"/>
+    <hyperlink ref="G33" r:id="rId60"/>
+    <hyperlink ref="F28" r:id="rId61"/>
+    <hyperlink ref="F29" r:id="rId62"/>
+    <hyperlink ref="F30" r:id="rId63"/>
+    <hyperlink ref="F31" r:id="rId64"/>
+    <hyperlink ref="F32" r:id="rId65"/>
+    <hyperlink ref="F33" r:id="rId66"/>
+    <hyperlink ref="G34" r:id="rId67"/>
+    <hyperlink ref="G35" r:id="rId68"/>
+    <hyperlink ref="G36" r:id="rId69"/>
+    <hyperlink ref="G37" r:id="rId70"/>
+    <hyperlink ref="G38" r:id="rId71"/>
+    <hyperlink ref="F34" r:id="rId72"/>
+    <hyperlink ref="F35" r:id="rId73"/>
+    <hyperlink ref="F36" r:id="rId74"/>
+    <hyperlink ref="F37" r:id="rId75"/>
+    <hyperlink ref="F38" r:id="rId76"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId77"/>
@@ -2476,8 +2476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>